<commit_message>
Revert China reorder to all brands
</commit_message>
<xml_diff>
--- a/data/input/China reorder.xlsx
+++ b/data/input/China reorder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nitesh\AM - Inventory replenishment\AM_Replenishment\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03FD05E-D10E-4906-9C77-6BBDE8A11617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16DEDD6-AE74-4A97-A016-EB5C74EA71BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6F3F26F-327D-42FE-B92F-B9D43C18F440}"/>
   </bookViews>
@@ -450,7 +450,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update avg weekly sales column + planning fix
</commit_message>
<xml_diff>
--- a/data/input/China reorder.xlsx
+++ b/data/input/China reorder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nitesh\AM - Inventory replenishment\AM_Replenishment\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16DEDD6-AE74-4A97-A016-EB5C74EA71BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049F5F58-6047-4A89-820E-CEDE5572B42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6F3F26F-327D-42FE-B92F-B9D43C18F440}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Avg</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Add Brand Filter across brands</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -450,7 +453,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,7 +538,9 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="K3" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="L3" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Setup env-based API base config
</commit_message>
<xml_diff>
--- a/data/input/China reorder.xlsx
+++ b/data/input/China reorder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nitesh\AM - Inventory replenishment\AM_Replenishment\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049F5F58-6047-4A89-820E-CEDE5572B42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2343C583-DEFE-4199-8C3E-220E7B572499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6F3F26F-327D-42FE-B92F-B9D43C18F440}"/>
   </bookViews>
@@ -453,7 +453,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update China Reorder thresholds + data changes
</commit_message>
<xml_diff>
--- a/data/input/China reorder.xlsx
+++ b/data/input/China reorder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nitesh\AM - Inventory replenishment\AM_Replenishment\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2343C583-DEFE-4199-8C3E-220E7B572499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B0E7E1-E3B8-46B0-B2FF-0645D29A6633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6F3F26F-327D-42FE-B92F-B9D43C18F440}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Avg</t>
   </si>
@@ -533,11 +533,19 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="K3" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
FC allocation logic update + governance + frontend sync
</commit_message>
<xml_diff>
--- a/data/input/China reorder.xlsx
+++ b/data/input/China reorder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nitesh\AM - Inventory replenishment\AM_Replenishment\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B0E7E1-E3B8-46B0-B2FF-0645D29A6633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72741B37-19FA-4803-A307-B7A3AFDCCFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6F3F26F-327D-42FE-B92F-B9D43C18F440}"/>
   </bookViews>
@@ -453,7 +453,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,7 +523,7 @@
       <c r="K2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Open Order aggregation fix and UI column update
</commit_message>
<xml_diff>
--- a/data/input/China reorder.xlsx
+++ b/data/input/China reorder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nitesh\AM - Inventory replenishment\AM_Replenishment\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72741B37-19FA-4803-A307-B7A3AFDCCFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1811E7E5-6B50-4E23-89A8-106D97F862B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6F3F26F-327D-42FE-B92F-B9D43C18F440}"/>
   </bookViews>
@@ -453,7 +453,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>